<commit_message>
#decentralizehk - DHK dao Team evidence A1-A6
</commit_message>
<xml_diff>
--- a/dhkgon/evidence.xlsx
+++ b/dhkgon/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonnip/Documents/gon-evidence/kldhk/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonnip/Documents/gon-evidence/dhkgon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAC1715-657B-CE41-8C2D-AB8EF693885C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841D96EE-2189-3549-80D3-733AA6C09FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="43">
   <si>
     <t>TxHash</t>
   </si>
@@ -79,24 +79,6 @@
     <t>nft id</t>
   </si>
   <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on irisnet</t>
-  </si>
-  <si>
-    <t>ibc class on dest chain</t>
-  </si>
-  <si>
-    <t>class id you issued</t>
-  </si>
-  <si>
-    <t>nft id you minted</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -143,13 +125,61 @@
   </si>
   <si>
     <t>omniflix15vsyx3fk9eqg3tmdp55m8gp77jvg9lee6ekr3y</t>
+  </si>
+  <si>
+    <t>874E4D4C201E86C8CA25EDAA0FF4BA9B2043624879109E8440D7C3BC550D3DA1</t>
+  </si>
+  <si>
+    <t>dhk</t>
+  </si>
+  <si>
+    <t>0F1C1ED97510DE62070D2D66B6DC2E7DAE1CEC92C60720607511DCC73BEF6F96</t>
+  </si>
+  <si>
+    <t>A7241B107D21087A4D44109CECFEEFBB7052C7D64B0CE5173A137619C8F4EA95</t>
+  </si>
+  <si>
+    <t>nf01</t>
+  </si>
+  <si>
+    <t>nft02</t>
+  </si>
+  <si>
+    <t>150D0552226FA487530BCA46E7ED0792F448FD8E8C54ECB2D548587AC9A77208</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>479EDA22ED16A9137CF0E2EF1F80CBB8816499E2BE357F13558DB3833D75D972</t>
+  </si>
+  <si>
+    <t>9F16792B2359530D5E7F3DE805490106E204C220DA8F21E98082EE12E734BD04</t>
+  </si>
+  <si>
+    <t>nft01</t>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>288E8F6C9684A18261E56B16799E798BEA09C0AA61A6570800CF84FF054F5A91</t>
+  </si>
+  <si>
+    <t>juno1vvdta627ndzrfwenedc0e0xmhc0wgn7x7yt6sw20894umvh37gpq00j0y8</t>
+  </si>
+  <si>
+    <t>931FDDCEA2DFA6CDC36AC3D711C3F26FB072A8716CE711618EC19B692BB563A9</t>
+  </si>
+  <si>
+    <t>ibc/9F16792B2359530D5E7F3DE805490106E204C220DA8F21E98082EE12E734BD04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +190,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -216,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -230,6 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,7 +574,7 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -555,54 +592,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1037,11 +1074,14 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1054,10 +1094,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1298,13 +1338,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1321,13 +1364,24 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1342,11 +1396,14 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1367,16 +1424,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1391,11 +1448,14 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1416,16 +1476,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1440,11 +1500,14 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1465,16 +1528,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1489,12 +1552,13 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="73.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1515,16 +1579,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stage2 - #decentralizehk - DHK DAO Team add A7-A20
</commit_message>
<xml_diff>
--- a/dhkgon/evidence.xlsx
+++ b/dhkgon/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonnip/Documents/gon-evidence/dhkgon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841D96EE-2189-3549-80D3-733AA6C09FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC55B52-0778-D14C-9C06-DA5851E57160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38240" yWindow="-3760" windowWidth="34060" windowHeight="19600" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="89">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -173,6 +158,159 @@
   </si>
   <si>
     <t>ibc/9F16792B2359530D5E7F3DE805490106E204C220DA8F21E98082EE12E734BD04</t>
+  </si>
+  <si>
+    <t>nft03</t>
+  </si>
+  <si>
+    <t>ibc/A5A33B838ED68D768D79D6881E67752B14BC05F3ADC25BF2E73E619F0B6C3BA5</t>
+  </si>
+  <si>
+    <t>ibc/72D1FED893066457E98E873187C0687DE6C15F6E91FEE1F507A598807183630F</t>
+  </si>
+  <si>
+    <t>nfta8</t>
+  </si>
+  <si>
+    <t>nfta92</t>
+  </si>
+  <si>
+    <t>ibc/BAAD0A4AD76974019BC5A30F6E7E02CA64FBD47B176255ABD8FBBC25C0118AC7</t>
+  </si>
+  <si>
+    <t>ibc/09FA076C3C26E675C40B4EAD26F3E0C6CE453F303835127634980A15C7F411C5</t>
+  </si>
+  <si>
+    <t>nfta10</t>
+  </si>
+  <si>
+    <t>nfta11</t>
+  </si>
+  <si>
+    <t>ibc/282A9225DDB30C16CB8FE052C2C987CACC1F71225A47B5E182E27367DB63410D</t>
+  </si>
+  <si>
+    <t>ibc/4F90C2EC8E8934F41A33617A33A43DD70BB86551F19BE7E018E411F7047BC652</t>
+  </si>
+  <si>
+    <t>nfta12</t>
+  </si>
+  <si>
+    <t>DA3C955FC3019F7580FBB4068832FEF8CBF341050D2FF0D1A3BC5001D7654B26</t>
+  </si>
+  <si>
+    <t>43A840B9C2B007B308D2DDFEBB5C08BA4E5ED401F3EE2D39D36FC11C2F4D5986</t>
+  </si>
+  <si>
+    <t>EE37F50D0413E3DC422A2864B58D153321953D620E73F30546A811997513FDD5</t>
+  </si>
+  <si>
+    <t>E3BAAB0B7AEFF6224486EC353E939D850E2899BB55390DC9F6D6E6D43F6771DB</t>
+  </si>
+  <si>
+    <t>ED9CAF39DED119AC359A7B6C68F16CACF8C8043F85ED721C10E69D5676F6E05D</t>
+  </si>
+  <si>
+    <t>6ADEC80E2C067172F19442E9C9453D08132DF9326AB6373114F0A95B2314C4FA</t>
+  </si>
+  <si>
+    <t>942B553A362108679E674E90AB8D80BC69EC2C0D0C25ED6B5453313E71A2DE6C</t>
+  </si>
+  <si>
+    <t>3A72B77C6CD4828AA36A8F626622F3313C10C517279AA82CCD59D966EB9BE28A</t>
+  </si>
+  <si>
+    <t>A28F0E5AFA84406B9BB1076B89205B1B08E01B9AA6B243AB29BF066F4313FBB2</t>
+  </si>
+  <si>
+    <t>F6966BABF64C87705C70E9DD48DF79D68C0B6C0836CEC8EC160207315154DB5D</t>
+  </si>
+  <si>
+    <t>752ED189D6A97C2E77559FBA0F9B9733B959BCDC449E77B55BB87D54A5771E0E</t>
+  </si>
+  <si>
+    <t>36B6733FB5659AA642A3738EE68AF8F4332D517B3BFCBC0CBADA4EA5736DB0CD</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>BAD599A16D2F241190B35F0932A63E65E5DB8455E0416D95645A4B7B3064CE2A</t>
+  </si>
+  <si>
+    <t>2224D4C44C70C1919424413DFFF6F3287E31F9C55252E87396A1D39A7C79768D</t>
+  </si>
+  <si>
+    <t>8F312ACDE3EF160851D11841284BF7A2635CE742A9050419967C28290753B9B9</t>
+  </si>
+  <si>
+    <t>916C9BBADD22D9919E54A32261703855E7761B219DE90C91A1ED62274D93619F</t>
+  </si>
+  <si>
+    <t>2C5C50E77F6B263651F77029D5AF1FB9570D42A6E92A88C668B21205F92A7498</t>
+  </si>
+  <si>
+    <t>D9B28B815A44F80BEC49EAE51CC7A8187E81FC8AEB86221329D16792D4450BAA</t>
+  </si>
+  <si>
+    <t>C667548982797BB4E5ED661E43AE32A8EA393053F02D9F9FEE5AD793E8B9B1C4</t>
+  </si>
+  <si>
+    <t>974746FD6368CBF78693AA74F3F3B9E10F3686D1831F9893EC3F0C2438C81EF7</t>
+  </si>
+  <si>
+    <t>CC2F72A60944D5ABE12C096579941ABF89218DABEAA388991E6EA99394194381</t>
+  </si>
+  <si>
+    <t>41D550E622EBC8A1FF4BD3310F5DDB4ECAFE49B4E83545A7D5ECF9F714894921</t>
+  </si>
+  <si>
+    <t>6ACD0B7954BE19D3DF552504F7A9E0264D4FB1420E6E554D27F7593B7BC019FC</t>
+  </si>
+  <si>
+    <t>FB3CA0DFD7CBA4AD2699E6AF9793C39E75F65756F21FBE264E473EE23A05A3D9</t>
+  </si>
+  <si>
+    <t>ED7991C8A56C3AE1961D79DCFF31A42F0D46EE08FAF683DD6461424E2F14271D</t>
+  </si>
+  <si>
+    <t>95A1D11DB574F8457496D7C3EAE69FD6829E660573CAAB00CFB2902CE1ADC8DF</t>
+  </si>
+  <si>
+    <t>9D96897E87410B1A47F50542AB8E1543A6085ADD7417946EA14AB2CAC2D0DF3F</t>
+  </si>
+  <si>
+    <t>BB4DEBE7825B05C5B6490438CEC22AD06C3428CC742F622F8F7DA1B24F4382D7</t>
+  </si>
+  <si>
+    <t>98BBD082C22A332A12B13F3149602CFBEDCC080B1E153B0803968DFFBFCE0592</t>
+  </si>
+  <si>
+    <t>662C0E5AE1BC4D4C8C977876506627773526E287A2308646F0A1E6E4A31EC778</t>
+  </si>
+  <si>
+    <t>5EC090519F299D805AFC381EBDFCA5DBFCFD93E14C0CC9D6091D9B52F1FEA57E</t>
+  </si>
+  <si>
+    <t>FDD9A9981254466C1952B77A0C4F25EA755E8D2979CD6131012F10BEF4434080</t>
+  </si>
+  <si>
+    <t>21CF06486815578881C80ED39BB3BEA71210620BB2051F5A0CFC112C13CF6C33</t>
+  </si>
+  <si>
+    <t>1CA84AC270BA683421B6D8C01F0BF84EFED822DA05FD23177BFC6DCA09DC2F4D</t>
+  </si>
+  <si>
+    <t>1DA32D37D819114882D08393697E0379938F3221E2394E17C46E4A6D49FE59E4</t>
+  </si>
+  <si>
+    <t>113C4D67E6F3A9CCD7B504CC06452BF7101E554E567C28D877C451D25C53249D</t>
   </si>
 </sst>
 </file>
@@ -252,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -267,6 +405,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,54 +733,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -654,28 +795,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="76.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -690,28 +833,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -726,28 +871,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="75.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -762,28 +909,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -796,13 +945,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -816,20 +967,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -842,13 +1007,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -862,24 +1029,39 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -888,13 +1070,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -908,20 +1092,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -934,13 +1132,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -954,20 +1154,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -980,13 +1194,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1000,20 +1216,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1026,13 +1256,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1046,20 +1278,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1089,15 +1335,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1110,13 +1356,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1130,20 +1378,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1156,13 +1434,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1176,20 +1456,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1356,32 +1666,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1413,10 +1723,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1424,16 +1734,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1465,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1476,16 +1786,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1517,10 +1827,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1528,16 +1838,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1552,7 +1862,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1568,10 +1878,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1579,16 +1889,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1603,28 +1913,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="75.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1639,28 +1951,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typo on A2 & A4
</commit_message>
<xml_diff>
--- a/dhkgon/evidence.xlsx
+++ b/dhkgon/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonnip/Documents/gon-evidence/dhkgon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC55B52-0778-D14C-9C06-DA5851E57160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFB3F8B-2CB5-214E-8E96-65ACBD371554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38240" yWindow="-3760" windowWidth="34060" windowHeight="19600" firstSheet="2" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38240" yWindow="-3760" windowWidth="34060" windowHeight="19600" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
   <si>
     <t>TxHash</t>
   </si>
@@ -124,9 +124,6 @@
     <t>A7241B107D21087A4D44109CECFEEFBB7052C7D64B0CE5173A137619C8F4EA95</t>
   </si>
   <si>
-    <t>nf01</t>
-  </si>
-  <si>
     <t>nft02</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
   </si>
   <si>
     <t>479EDA22ED16A9137CF0E2EF1F80CBB8816499E2BE357F13558DB3833D75D972</t>
-  </si>
-  <si>
-    <t>9F16792B2359530D5E7F3DE805490106E204C220DA8F21E98082EE12E734BD04</t>
   </si>
   <si>
     <t>nft01</t>
@@ -390,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -405,9 +399,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,10 +806,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -853,10 +844,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -891,10 +882,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -929,10 +920,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -967,34 +958,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1029,34 +1020,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1092,34 +1083,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1154,34 +1145,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1216,34 +1207,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1278,34 +1269,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>76</v>
+      <c r="A5" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1378,50 +1369,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1436,7 +1427,7 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1456,50 +1447,50 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1650,8 +1641,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1680,7 +1671,7 @@
         <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1691,7 +1682,7 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1734,16 +1725,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1759,7 +1750,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1786,16 +1777,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1838,16 +1829,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1889,16 +1880,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1933,10 +1924,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1971,10 +1962,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stage3 - #decentralizehk - DHK DAO Team add B1,B2
</commit_message>
<xml_diff>
--- a/dhkgon/evidence.xlsx
+++ b/dhkgon/evidence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonnip/Documents/gon-evidence/dhkgon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFB3F8B-2CB5-214E-8E96-65ACBD371554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F107F308-3324-9A4F-92A7-A82F592C0E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38240" yWindow="-3760" windowWidth="34060" windowHeight="19600" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38240" yWindow="-3760" windowWidth="34060" windowHeight="19600" firstSheet="5" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
   <si>
     <t>TxHash</t>
   </si>
@@ -305,6 +305,18 @@
   </si>
   <si>
     <t>113C4D67E6F3A9CCD7B504CC06452BF7101E554E567C28D877C451D25C53249D</t>
+  </si>
+  <si>
+    <t>EDE966069018848F2197B32E36201EA929B9874E2F8665C5479F0AEE4B2238EE</t>
+  </si>
+  <si>
+    <t>19EAA845F7BC4FBF5433FF5B57004D90F82B3029BA604BC3F133B26CEE02CB95</t>
+  </si>
+  <si>
+    <t>A5C7DDC781BCF293A7C90F06F99EBCAD0CC93C99058C3E45578E1381A3E2D703</t>
+  </si>
+  <si>
+    <t>C46E33153B5827ADF15DDFFF86ABD3376607C8EFEA5AAA35FD90EC0306DB90B4</t>
   </si>
 </sst>
 </file>
@@ -1505,6 +1517,78 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="70.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1532,8 +1616,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1566,74 +1650,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
@@ -1641,7 +1657,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Stage3 - #decentralizehk - DHK DAO Team add B5-B7
</commit_message>
<xml_diff>
--- a/dhkgon/evidence.xlsx
+++ b/dhkgon/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonnip/Documents/gon-evidence/dhkgon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F107F308-3324-9A4F-92A7-A82F592C0E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1887184-50C3-D243-B88F-DFA0ED396E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38240" yWindow="-3760" windowWidth="34060" windowHeight="19600" firstSheet="5" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" firstSheet="10" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,23 +38,18 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
-  </si>
-  <si>
     <t>ChainID</t>
   </si>
   <si>
@@ -317,6 +312,24 @@
   </si>
   <si>
     <t>C46E33153B5827ADF15DDFFF86ABD3376607C8EFEA5AAA35FD90EC0306DB90B4</t>
+  </si>
+  <si>
+    <t>1D6EE65F9E4D815207BE00932854E2CBDDDCE9B4067B3CA5E26AD1A3468B3EC4</t>
+  </si>
+  <si>
+    <t>4A35DD599968E46123EC76E1E5AFE3648278A590FE8730F3BB231944D316AFD5</t>
+  </si>
+  <si>
+    <t>8A2440A75968A192FDE40B47285F45AF610017200F1DA3284173BC298916B840</t>
+  </si>
+  <si>
+    <t>DB3B950CF257ADDC73658282778746A8B62C30190EE6E002AC532994B8F1FB04</t>
+  </si>
+  <si>
+    <t>E3DA746A1D3D9F3EBDDC20E0B849439823787FB1D9D90304B419B23BA3E1CE03</t>
+  </si>
+  <si>
+    <t>DCF5671B22E5896BB17B785B1A200BBC4134C1FCA12CAA434C59487CA9DEDFE6</t>
   </si>
 </sst>
 </file>
@@ -736,54 +749,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -810,18 +823,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -848,18 +861,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -886,18 +899,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -924,18 +937,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -965,39 +978,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1027,39 +1040,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1090,39 +1103,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1152,39 +1165,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1214,39 +1227,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1276,39 +1289,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1338,15 +1351,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1376,55 +1389,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1454,55 +1467,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1517,7 +1530,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -1532,6 +1545,42 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
@@ -1546,20 +1595,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="73.6640625" bestFit="1" customWidth="1"/>
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="73.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,18 +1631,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <sheetView zoomScale="114" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="70.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1603,46 +1654,45 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF61869-5B89-7E4A-9D4B-566A4C8AD5A6}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="71.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1673,32 +1723,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1730,27 +1780,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1782,27 +1832,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1834,27 +1884,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1885,27 +1935,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1932,18 +1982,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1970,18 +2020,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>